<commit_message>
update in images + slipt the css and js to files
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>backlog</t>
   </si>
@@ -43,7 +43,7 @@
     <t>create html page</t>
   </si>
   <si>
-    <t>yoni</t>
+    <t>yaron</t>
   </si>
   <si>
     <t>done</t>
@@ -52,7 +52,7 @@
     <t>TTN-2</t>
   </si>
   <si>
-    <t>create commants list</t>
+    <t>create commands list</t>
   </si>
   <si>
     <t>moshe</t>
@@ -64,7 +64,7 @@
     <t>add copy to clipboard</t>
   </si>
   <si>
-    <t>inProgress</t>
+    <t>InProgress</t>
   </si>
   <si>
     <t>TTN-4</t>
@@ -85,6 +85,9 @@
     <t>add login/  signup</t>
   </si>
   <si>
+    <t>open</t>
+  </si>
+  <si>
     <t>TTN-7</t>
   </si>
   <si>
@@ -130,14 +133,14 @@
     <t>wating for approval</t>
   </si>
   <si>
-    <t>approved/ merged</t>
+    <t>approved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -165,6 +168,10 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -286,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -321,9 +328,15 @@
     <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
@@ -334,7 +347,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -648,7 +661,7 @@
       <c r="E7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="13">
@@ -688,11 +701,11 @@
       <c r="E9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="13">
-        <v>3.0</v>
+      <c r="G9" s="14">
+        <v>2.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -705,55 +718,57 @@
       <c r="D10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13">
-        <v>2.0</v>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="14">
+        <v>4.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
       <c r="G11" s="13">
         <v>2.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="B12" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="D12" s="16"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="13">
-        <v>3.0</v>
-      </c>
+      <c r="G12" s="17"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
+        <v>29</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="13"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="B14" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -763,7 +778,7 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -773,7 +788,7 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -783,7 +798,7 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -793,7 +808,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="B18" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -803,7 +818,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="B19" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -813,7 +828,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="B20" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -823,31 +838,35 @@
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="F22" s="18" t="s">
-        <v>36</v>
+      <c r="F22" s="20" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="F23" s="19" t="s">
-        <v>37</v>
+      <c r="F23" s="21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="F27" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" ht="15.75" customHeight="1"/>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>

</xml_diff>